<commit_message>
bug fix : FixXML , heder->header
</commit_message>
<xml_diff>
--- a/test/TIDL.xlsx
+++ b/test/TIDL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\code\lg\TIDL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\code\github\CGA_RDL\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="25596" windowHeight="14976" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
   <si>
     <t>type</t>
   </si>
@@ -487,9 +487,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">uint8_t* </t>
-  </si>
-  <si>
     <t>ARG1</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -507,6 +504,148 @@
   </si>
   <si>
     <t>[HEADER]Arguments</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>did</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>len</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>att</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ame</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ype</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint16_t</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint8_t</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint16_t</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint16_t</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint8_t</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint8_t*</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>escription</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc len</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc did</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc att</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc data</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>init</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>NULL</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>`          android::sp&lt;Buffer&gt; buf = new Buffer();
+            buf-&gt;setSize(len);
+            data.read(buf-&gt;data(), len);</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[HEADER]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>xx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t>Data</t>
+    </r>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -644,7 +783,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -665,6 +804,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -728,7 +870,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1072,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1254,13 +1396,13 @@
         <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
@@ -1443,21 +1585,21 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1465,7 +1607,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1479,7 +1621,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1629,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
@@ -1495,7 +1637,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
@@ -1503,7 +1645,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>19</v>
       </c>
@@ -1511,7 +1653,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>22</v>
       </c>
@@ -1522,7 +1664,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1672,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
@@ -1541,7 +1683,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>27</v>
       </c>
@@ -1550,6 +1692,160 @@
       </c>
       <c r="C59" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A62" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>55</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="96" x14ac:dyDescent="0.45">
+      <c r="A74" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="175.2" x14ac:dyDescent="0.45">
+      <c r="A75" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1559,7 +1855,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$5:$A$98</xm:f>
@@ -1583,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E14"/>
+  <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1596,9 +1892,9 @@
     <col min="3" max="3" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
@@ -1607,22 +1903,22 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1633,7 +1929,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>62</v>
       </c>
@@ -1644,7 +1940,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="132" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" ht="132" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>67</v>
       </c>
@@ -1655,22 +1951,18 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1686,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E4"/>
+  <dimension ref="A4:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="A4" sqref="A4:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1697,21 +1989,74 @@
     <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1725,7 +2070,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$5:$A$98</xm:f>
           </x14:formula1>
-          <xm:sqref>B4:P4</xm:sqref>
+          <xm:sqref>E4:P4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
bug fix of 1_excel.pl & add function  stcI_FILE_LOWER : YES   stcI_ALL_LOWER : YES
1. stcI_FILE_LOWER : YES   -> change file name into lower case
2. stcI_ALL_LOWER : YES    -> change all filename including direcotry  into lower case
</commit_message>
<xml_diff>
--- a/test/TIDL.xlsx
+++ b/test/TIDL.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="101">
   <si>
     <t>type</t>
   </si>
@@ -616,16 +616,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>`          android::sp&lt;Buffer&gt; buf = new Buffer();
-            buf-&gt;setSize(len);
-            data.read(buf-&gt;data(), len);</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>[HEADER]</t>
     </r>
@@ -646,6 +636,22 @@
       </rPr>
       <t>Data</t>
     </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>diagnostic module</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARG1</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>[HEADER]name</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1216,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1237,6 +1243,9 @@
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
       <c r="C1" s="1"/>
       <c r="F1" s="2"/>
       <c r="H1" s="1"/>
@@ -1244,6 +1253,9 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
       </c>
       <c r="C2" s="1"/>
       <c r="F2" s="1"/>
@@ -1589,8 +1601,8 @@
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>72</v>
+      <c r="B49" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>73</v>
@@ -1696,10 +1708,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>82</v>
@@ -1821,7 +1833,7 @@
         <v>62</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C74" s="10" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
auto arguments and member variable genertion
</commit_message>
<xml_diff>
--- a/test/TIDL.xlsx
+++ b/test/TIDL.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="108">
   <si>
     <t>type</t>
   </si>
@@ -616,6 +616,10 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
+    <t>name</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>[HEADER]</t>
     </r>
@@ -651,7 +655,41 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>[HEADER]name</t>
+    <t>Len</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataLen</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>writeInt32</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>writeByteArray</t>
+  </si>
+  <si>
+    <r>
+      <t>[HEADER]Ar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>gType1</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>readInt32</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>kkk</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1222,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1244,7 +1282,7 @@
         <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1"/>
       <c r="F1" s="2"/>
@@ -1255,7 +1293,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1"/>
       <c r="F2" s="1"/>
@@ -1597,12 +1635,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>73</v>
@@ -1611,7 +1649,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -1619,7 +1657,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1633,7 +1671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1641,7 +1679,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
@@ -1649,7 +1687,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
@@ -1657,7 +1695,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>19</v>
       </c>
@@ -1665,7 +1703,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>22</v>
       </c>
@@ -1676,7 +1714,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>24</v>
       </c>
@@ -1684,7 +1722,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
@@ -1695,7 +1733,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>27</v>
       </c>
@@ -1706,12 +1744,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>82</v>
@@ -1720,10 +1758,13 @@
         <v>94</v>
       </c>
       <c r="E62" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F62" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>1</v>
       </c>
@@ -1736,16 +1777,16 @@
       <c r="D63">
         <v>0</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="C64" t="s">
         <v>86</v>
@@ -1753,11 +1794,11 @@
       <c r="D64">
         <v>0</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>3</v>
       </c>
@@ -1770,11 +1811,11 @@
       <c r="D65">
         <v>0</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>4</v>
       </c>
@@ -1788,12 +1829,15 @@
         <v>95</v>
       </c>
       <c r="E66" t="s">
+        <v>102</v>
+      </c>
+      <c r="F66" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A69" s="1" t="s">
-        <v>76</v>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="B69" t="s">
         <v>64</v>
@@ -1802,33 +1846,39 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B72" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>55</v>
       </c>
-      <c r="B73" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="96" x14ac:dyDescent="0.45">
+      <c r="B73" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="96" x14ac:dyDescent="0.45">
       <c r="A74" s="5" t="s">
         <v>62</v>
       </c>
@@ -1839,7 +1889,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="175.2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" ht="175.2" x14ac:dyDescent="0.45">
       <c r="A75" s="7" t="s">
         <v>67</v>
       </c>
@@ -1847,17 +1897,29 @@
         <v>68</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B76" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>84</v>
+      </c>
+      <c r="B77" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 1_excel.pl : add {NOHEADER}  {HEADER} to seperate between HEADER and no HEADER
</commit_message>
<xml_diff>
--- a/test/TIDL.xlsx
+++ b/test/TIDL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4200" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="4800" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,13 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="108">
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>name1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="104">
   <si>
     <t>O</t>
   </si>
@@ -43,12 +37,6 @@
     <t>DID_WORK_FOR_DEFINE_1</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>name2</t>
-  </si>
-  <si>
     <t>wishtoUseAPI_2</t>
   </si>
   <si>
@@ -61,9 +49,6 @@
     <t>DID_WORK_FOR_DEFINE_2</t>
   </si>
   <si>
-    <t>name3</t>
-  </si>
-  <si>
     <t>wishtoUseAPI_3</t>
   </si>
   <si>
@@ -115,9 +100,6 @@
     <t>DID_WORK_FOR_DEFINE_9</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>Diag</t>
   </si>
   <si>
@@ -130,9 +112,6 @@
     <t>[HEADER]Function</t>
   </si>
   <si>
-    <t>[HEADER]CLASSL_MEMBER_VAR</t>
-  </si>
-  <si>
     <t>[HEADER]Related_Manager</t>
   </si>
   <si>
@@ -140,7 +119,7 @@
   </si>
   <si>
     <t>usingName</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -155,7 +134,7 @@
       </rPr>
       <t>MI</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -170,7 +149,7 @@
       </rPr>
       <t>ystem</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -185,7 +164,7 @@
       </rPr>
       <t>oc</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -200,31 +179,31 @@
       </rPr>
       <t>udio</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>vif</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>onReceiver</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>[HEADER]Receiver</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>interfaceFunction</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>onSite</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>BnReceiverClass</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>BnvifManagerReceiver</t>
@@ -237,63 +216,51 @@
   </si>
   <si>
     <t>wishtoUseAPI_1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>DID_WORK_FOR_DEFINE_0</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>uint32_t</t>
   </si>
   <si>
     <t>uint32_t</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>int32_t</t>
   </si>
   <si>
     <t>int32_t</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Data</t>
   </si>
   <si>
     <t>Data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>void</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>void</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>void</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>android::sp&lt;Buffer&gt;</t>
   </si>
   <si>
     <t>uint32_t ??? = parcel.readInt32();</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>read</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>write</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -332,7 +299,7 @@
       </rPr>
       <t xml:space="preserve">* </t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">    size_t arrayLength = static_cast&lt;uint32_t&gt;(parcel.readInt32());
@@ -342,7 +309,7 @@
     uint8_t * copyBytes = new uint8_t[arrayLength];
     if (bytes != NULL)
         memcpy (copyBytes,bytes,arrayLength);</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -478,49 +445,49 @@
   <si>
     <t xml:space="preserve">       (void)data.writeInt32(buf-&gt;size());
         (void)data.write(buf-&gt;data(), buf-&gt;size());</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">          android::sp&lt;Buffer&gt; buf = new Buffer();
             buf-&gt;setSize(len);
             data.read(buf-&gt;data(), len);</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>ARG1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>ARG2</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>ARG3</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>[HEADER]Data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>[HEADER]Arguments</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>did</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>len</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>att</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -535,7 +502,7 @@
       </rPr>
       <t>ame</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -550,31 +517,31 @@
       </rPr>
       <t>ype</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>uint16_t</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>uint8_t</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>uint16_t</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>uint16_t</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>uint8_t</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>uint8_t*</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -589,35 +556,35 @@
       </rPr>
       <t>escription</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>desc len</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>desc did</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>desc att</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>desc data</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>init</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>NULL</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -637,34 +604,27 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Courier New"/>
+        <family val="3"/>
       </rPr>
       <t>Data</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>diagnostic module</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>ARG1</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>Len</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>dataLen</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>writeInt32</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>writeByteArray</t>
@@ -682,22 +642,63 @@
       </rPr>
       <t>gType1</t>
     </r>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>readInt32</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>kkk</t>
-    <phoneticPr fontId="6" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>rom</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint32_t</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc int32</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxData</t>
+  </si>
+  <si>
+    <t>xxData</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>uint8_t</t>
+  </si>
+  <si>
+    <r>
+      <t>[HEADER]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>Multi</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>[HEADER]read</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -706,14 +707,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -814,42 +811,41 @@
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -887,13 +883,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -914,7 +910,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1258,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1277,670 +1273,589 @@
     <col min="10" max="10" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1"/>
       <c r="F1" s="2"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1"/>
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="C5" s="1"/>
       <c r="F5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="C6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>74</v>
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>54</v>
+        <v>10</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" t="s">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>52</v>
+        <v>3</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
+        <v>36</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50">
         <v>2</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51" s="1" t="s">
+      <c r="A51">
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" t="s">
-        <v>54</v>
+        <v>77</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
-        <v>9</v>
+      <c r="A52">
+        <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" t="s">
+        <v>90</v>
+      </c>
+      <c r="F52" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A53" s="1" t="s">
-        <v>13</v>
+      <c r="A53">
+        <v>5</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" t="s">
-        <v>60</v>
+        <v>96</v>
+      </c>
+      <c r="C53" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A56" s="1" t="s">
-        <v>22</v>
+      <c r="A56" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" t="s">
-        <v>54</v>
+      <c r="A57" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A58" s="1" t="s">
-        <v>26</v>
+      <c r="A58" t="s">
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C58" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A59" s="1" t="s">
-        <v>27</v>
+      <c r="A59" t="s">
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="96" x14ac:dyDescent="0.45">
+      <c r="A60" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="B60" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="175.2" x14ac:dyDescent="0.45">
+      <c r="A61" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A62" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D62" s="4" t="s">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" t="s">
         <v>94</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>89</v>
+      <c r="C62" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A63">
-        <v>1</v>
+      <c r="A63" t="s">
+        <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="F63" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A64">
-        <v>2</v>
-      </c>
-      <c r="B64" t="s">
-        <v>107</v>
-      </c>
-      <c r="C64" t="s">
-        <v>86</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="F64" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A65">
-        <v>3</v>
-      </c>
-      <c r="B65" t="s">
-        <v>79</v>
-      </c>
-      <c r="C65" t="s">
-        <v>87</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="F65" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A66">
-        <v>4</v>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="B66" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
-      </c>
-      <c r="D66" t="s">
-        <v>95</v>
-      </c>
-      <c r="E66" t="s">
-        <v>102</v>
-      </c>
-      <c r="F66" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B69" t="s">
-        <v>64</v>
-      </c>
-      <c r="C69" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>53</v>
-      </c>
-      <c r="B72" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
         <v>55</v>
       </c>
-      <c r="B73" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="96" x14ac:dyDescent="0.45">
-      <c r="A74" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B74" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="175.2" x14ac:dyDescent="0.45">
-      <c r="A75" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" t="s">
-        <v>106</v>
-      </c>
-      <c r="C76" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>84</v>
-      </c>
-      <c r="B77" t="s">
-        <v>106</v>
-      </c>
-      <c r="C77" t="s">
-        <v>103</v>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36:D45 B12:D19">
+      <formula1>$A$57:$A$63</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$5:$A$98</xm:f>
           </x14:formula1>
-          <xm:sqref>C50:L59 C26:L34</xm:sqref>
+          <xm:sqref>E36:L45 E12:L20 C20:D20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B50:B59 B26:B34</xm:sqref>
+          <xm:sqref>B20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1968,78 +1883,78 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>66</v>
+        <v>48</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>70</v>
+      <c r="A7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="132" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>69</v>
+      <c r="A8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14:E14">
       <formula1>$A$5:$A$98</formula1>
@@ -2065,16 +1980,16 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>89</v>
+        <v>65</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -2082,13 +1997,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -2096,13 +2011,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -2110,13 +2025,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -2124,17 +2039,17 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>